<commit_message>
fixed the validation page
</commit_message>
<xml_diff>
--- a/DMP/Report/Template/ART sites.xlsx
+++ b/DMP/Report/Template/ART sites.xlsx
@@ -8133,8 +8133,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E1172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1153" workbookViewId="0">
-      <selection activeCell="B1173" sqref="B1173"/>
+    <sheetView tabSelected="1" topLeftCell="A1163" workbookViewId="0">
+      <selection activeCell="B1169" sqref="B1169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Corrected DQA upload for UMB and Partner
</commit_message>
<xml_diff>
--- a/DMP/Report/Template/ART sites.xlsx
+++ b/DMP/Report/Template/ART sites.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4686" uniqueCount="2564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4686" uniqueCount="2563">
   <si>
     <t>Facility</t>
   </si>
@@ -7693,9 +7693,6 @@
   </si>
   <si>
     <t>xu4mnSBhh65</t>
-  </si>
-  <si>
-    <t>Primary Health Centre Arumangye Bosco</t>
   </si>
   <si>
     <t>Arumangye Bosco Primary Health Center</t>
@@ -7725,7 +7722,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -7817,7 +7814,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -8129,12 +8126,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E1172"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1163" workbookViewId="0">
-      <selection activeCell="B1169" sqref="B1169"/>
+      <selection activeCell="B1171" sqref="B1171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -24383,7 +24380,7 @@
         <v>2453</v>
       </c>
       <c r="B1160" s="3" t="s">
-        <v>2561</v>
+        <v>2560</v>
       </c>
       <c r="C1160" s="3" t="s">
         <v>2526</v>
@@ -24526,10 +24523,10 @@
         <v>2555</v>
       </c>
       <c r="C1170" t="s">
+        <v>2555</v>
+      </c>
+      <c r="D1170" t="s">
         <v>2556</v>
-      </c>
-      <c r="D1170" t="s">
-        <v>2557</v>
       </c>
     </row>
     <row r="1171" spans="1:4" x14ac:dyDescent="0.35">
@@ -24537,13 +24534,13 @@
         <v>2453</v>
       </c>
       <c r="B1171" t="s">
+        <v>2557</v>
+      </c>
+      <c r="C1171" t="s">
         <v>2558</v>
       </c>
-      <c r="C1171" t="s">
+      <c r="D1171" t="s">
         <v>2559</v>
-      </c>
-      <c r="D1171" t="s">
-        <v>2560</v>
       </c>
     </row>
     <row r="1172" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -24551,13 +24548,13 @@
         <v>790</v>
       </c>
       <c r="B1172" s="6" t="s">
-        <v>2563</v>
+        <v>2562</v>
       </c>
       <c r="C1172" s="6" t="s">
-        <v>2563</v>
+        <v>2562</v>
       </c>
       <c r="D1172" s="6" t="s">
-        <v>2562</v>
+        <v>2561</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor dqa q3 corrections
</commit_message>
<xml_diff>
--- a/DMP/Report/Template/ART sites.xlsx
+++ b/DMP/Report/Template/ART sites.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7940" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7940" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <definedName name="LGA">[1]MainPage!$S$17</definedName>
     <definedName name="LGAFac_list">[1]!LGAFac[#Headers]</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" iterate="1" iterateCount="1" iterateDelta="1E-4"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11152" uniqueCount="6046">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11392" uniqueCount="6188">
   <si>
     <t>Facility</t>
   </si>
@@ -18179,6 +18179,432 @@
   </si>
   <si>
     <t>FBBTY7S1T4S</t>
+  </si>
+  <si>
+    <t>fc Kuchibuyi Primary Health Center</t>
+  </si>
+  <si>
+    <t>MjPJsyoDyUI</t>
+  </si>
+  <si>
+    <t>Gombe</t>
+  </si>
+  <si>
+    <t>go Akko</t>
+  </si>
+  <si>
+    <t>go Bogo Model Primary Health Center</t>
+  </si>
+  <si>
+    <t>hnu8aVM6eMV</t>
+  </si>
+  <si>
+    <t>go Balanga</t>
+  </si>
+  <si>
+    <t>go Cham Primary Health Center</t>
+  </si>
+  <si>
+    <t>tIEFDNyv2IV</t>
+  </si>
+  <si>
+    <t>go Billiri</t>
+  </si>
+  <si>
+    <t>go Pobaure Primary Health Center</t>
+  </si>
+  <si>
+    <t>frnHxx8ZcTF</t>
+  </si>
+  <si>
+    <t>go Funakaye</t>
+  </si>
+  <si>
+    <t>go Jalingo Primary Health Center</t>
+  </si>
+  <si>
+    <t>I9vA78jcthr</t>
+  </si>
+  <si>
+    <t>go Gombe</t>
+  </si>
+  <si>
+    <t>go Bolari Maternal and Child Health Clinic</t>
+  </si>
+  <si>
+    <t>ve4UhhWPdtv</t>
+  </si>
+  <si>
+    <t>go Herwagana Maternal and Child Health Clinic</t>
+  </si>
+  <si>
+    <t>TinjgNiJrB4</t>
+  </si>
+  <si>
+    <t>go Kasuwan Mata Health Clinic</t>
+  </si>
+  <si>
+    <t>y6Kk5VUXOX7</t>
+  </si>
+  <si>
+    <t>go London Maidorawa Health Clinic</t>
+  </si>
+  <si>
+    <t>oso9UXCPxTW</t>
+  </si>
+  <si>
+    <t>go Nasarawo Maternal and Child Health Clinic</t>
+  </si>
+  <si>
+    <t>tRkbi8NqKzg</t>
+  </si>
+  <si>
+    <t>go Pantami Primary Health Center</t>
+  </si>
+  <si>
+    <t>pU92ZUAY68L</t>
+  </si>
+  <si>
+    <t>go Sunnah Hospital</t>
+  </si>
+  <si>
+    <t>TiAwIXFMkLy</t>
+  </si>
+  <si>
+    <t>go Town Maternity Gombe</t>
+  </si>
+  <si>
+    <t>aGOQB2fZ1Bt</t>
+  </si>
+  <si>
+    <t>go Tudun Wada Primary Health Center</t>
+  </si>
+  <si>
+    <t>dxf5N2oFePK</t>
+  </si>
+  <si>
+    <t>go Kwami</t>
+  </si>
+  <si>
+    <t>go Daban Fulani Maternal and Child Health Clinic</t>
+  </si>
+  <si>
+    <t>K4zAO0M2Kmq</t>
+  </si>
+  <si>
+    <t>kd Chikun</t>
+  </si>
+  <si>
+    <t>kd Kasuwa Magani Primary Health Center</t>
+  </si>
+  <si>
+    <t>JWZaYKHTAvt</t>
+  </si>
+  <si>
+    <t>kd Kujama Primary Health Center</t>
+  </si>
+  <si>
+    <t>nwcnPbXH2SR</t>
+  </si>
+  <si>
+    <t>kd Nasarawa Primary Health Center</t>
+  </si>
+  <si>
+    <t>qq4e0kfaUvb</t>
+  </si>
+  <si>
+    <t>kd Romi Primary Health Center</t>
+  </si>
+  <si>
+    <t>FLqvfq0KBA4</t>
+  </si>
+  <si>
+    <t>kd Igabi</t>
+  </si>
+  <si>
+    <t>kd Mararaban Jos Primary Health Center</t>
+  </si>
+  <si>
+    <t>OKrnMlZFkFf</t>
+  </si>
+  <si>
+    <t>kd Barde Primary Health Center</t>
+  </si>
+  <si>
+    <t>nnO4MwYN93D</t>
+  </si>
+  <si>
+    <t>kd Gidan Waya Primary Health Center</t>
+  </si>
+  <si>
+    <t>zDhjewQr48h</t>
+  </si>
+  <si>
+    <t>kd Godogodo Primary Health Center</t>
+  </si>
+  <si>
+    <t>gOO2jNM0enh</t>
+  </si>
+  <si>
+    <t>kd Jagindi Tasha Health Clinic</t>
+  </si>
+  <si>
+    <t>Md3GGdU4n1S</t>
+  </si>
+  <si>
+    <t>kd Salem Medical Center - Kafanchan</t>
+  </si>
+  <si>
+    <t>f0wy9MgKtUx</t>
+  </si>
+  <si>
+    <t>kd Kaduna North</t>
+  </si>
+  <si>
+    <t>kd Al-Munnir Hospital</t>
+  </si>
+  <si>
+    <t>vpRIpHsK1EG</t>
+  </si>
+  <si>
+    <t>kd Hayin Banki Primary Health Center</t>
+  </si>
+  <si>
+    <t>V5Le2Ban78U</t>
+  </si>
+  <si>
+    <t>kd Tukur Malali Primary Health Center</t>
+  </si>
+  <si>
+    <t>Gh18S2BxHKn</t>
+  </si>
+  <si>
+    <t>kd Ungwan Shanu Primary Health Center</t>
+  </si>
+  <si>
+    <t>hD3xRpPBnWf</t>
+  </si>
+  <si>
+    <t>kd Kaduna South</t>
+  </si>
+  <si>
+    <t>kd Kudenda Primary Health Center</t>
+  </si>
+  <si>
+    <t>Xs1MosdNYO5</t>
+  </si>
+  <si>
+    <t>kd Kurmi Mashi Primary Health Center</t>
+  </si>
+  <si>
+    <t>oB3NepeAtXB</t>
+  </si>
+  <si>
+    <t>kd Television Primary Health Center</t>
+  </si>
+  <si>
+    <t>zVAiLsWRBQb</t>
+  </si>
+  <si>
+    <t>kd Tudun Wada Family Health Unit</t>
+  </si>
+  <si>
+    <t>BTfKBTk1iJ9</t>
+  </si>
+  <si>
+    <t>kd Kagarko</t>
+  </si>
+  <si>
+    <t>kd Jere Primary Health Center</t>
+  </si>
+  <si>
+    <t>k9ShWQ2CK5c</t>
+  </si>
+  <si>
+    <t>kd Kagarko Primary Health Center</t>
+  </si>
+  <si>
+    <t>pyCjMH0xPyt</t>
+  </si>
+  <si>
+    <t>kd Taffa Health Center</t>
+  </si>
+  <si>
+    <t>uDPDgMxSdDU</t>
+  </si>
+  <si>
+    <t>kd Kauru</t>
+  </si>
+  <si>
+    <t>kd Damakasuwa Health Clinic</t>
+  </si>
+  <si>
+    <t>HneMVa1g1rl</t>
+  </si>
+  <si>
+    <t>kd Kubau</t>
+  </si>
+  <si>
+    <t>kd Anchau Primary Health Center</t>
+  </si>
+  <si>
+    <t>bWhHCsWrqie</t>
+  </si>
+  <si>
+    <t>kd Lere</t>
+  </si>
+  <si>
+    <t>kd Evangelical Church of West Africa (ECWA) Comprehensive Health Center - Ungwan Bawa</t>
+  </si>
+  <si>
+    <t>IO38n1uX0Z7</t>
+  </si>
+  <si>
+    <t>kd Garun Kurama Primary Health Center</t>
+  </si>
+  <si>
+    <t>XyGNdts89ji</t>
+  </si>
+  <si>
+    <t>kd Lere Primary Health Center</t>
+  </si>
+  <si>
+    <t>Eq0SMoSZuRc</t>
+  </si>
+  <si>
+    <t>kd Ramin Kura Primary Health Center</t>
+  </si>
+  <si>
+    <t>FIyoBlcRtsm</t>
+  </si>
+  <si>
+    <t>kd Makarfi</t>
+  </si>
+  <si>
+    <t>kd Makarfi Primary Health Center</t>
+  </si>
+  <si>
+    <t>uEhcBbwErng</t>
+  </si>
+  <si>
+    <t>kd Sanga</t>
+  </si>
+  <si>
+    <t>kd Combila Health Center</t>
+  </si>
+  <si>
+    <t>GDk0Y7jIeAz</t>
+  </si>
+  <si>
+    <t>kd Gwantu Primary Health Center</t>
+  </si>
+  <si>
+    <t>HwVtJkZK6mX</t>
+  </si>
+  <si>
+    <t>kd Karshi Daji Health Center</t>
+  </si>
+  <si>
+    <t>hduP3AR3vqA</t>
+  </si>
+  <si>
+    <t>kd Mayir Primary Health Center</t>
+  </si>
+  <si>
+    <t>iY9AWY5Juy5</t>
+  </si>
+  <si>
+    <t>kd Nimbe Health Center</t>
+  </si>
+  <si>
+    <t>tVjg7MfEpfY</t>
+  </si>
+  <si>
+    <t>Kogi</t>
+  </si>
+  <si>
+    <t>ko Adavi</t>
+  </si>
+  <si>
+    <t>ko Aimoizza Clinic</t>
+  </si>
+  <si>
+    <t>oyiQ8ltpF2c</t>
+  </si>
+  <si>
+    <t>ko Ogaminana Clinic - Adavi</t>
+  </si>
+  <si>
+    <t>e5aGNsUPSvn</t>
+  </si>
+  <si>
+    <t>ko Ankpa</t>
+  </si>
+  <si>
+    <t>ko Ankpa Primary Health Center</t>
+  </si>
+  <si>
+    <t>DaTMu3rYeQK</t>
+  </si>
+  <si>
+    <t>ko Bethel Hospital</t>
+  </si>
+  <si>
+    <t>N2YrIzbDRkx</t>
+  </si>
+  <si>
+    <t>ko Emere Primary Health Center</t>
+  </si>
+  <si>
+    <t>wHuOS6cG6Sr</t>
+  </si>
+  <si>
+    <t>ko Living Hope Hospital</t>
+  </si>
+  <si>
+    <t>CFi2osDSAQt</t>
+  </si>
+  <si>
+    <t>ko Dekina</t>
+  </si>
+  <si>
+    <t>ko Ayingba Comprehensive Health Center</t>
+  </si>
+  <si>
+    <t>WwVbcxjtu79</t>
+  </si>
+  <si>
+    <t>ko St. Luke's Clinic - Egume</t>
+  </si>
+  <si>
+    <t>HrGggd9x1os</t>
+  </si>
+  <si>
+    <t>ko Igalamela-Odolu</t>
+  </si>
+  <si>
+    <t>ko Ajaka Primary Health Center</t>
+  </si>
+  <si>
+    <t>g6NVwIeNfgD</t>
+  </si>
+  <si>
+    <t>ko Kogi</t>
+  </si>
+  <si>
+    <t>ko Ideal Hospital - Koton-Karfe</t>
+  </si>
+  <si>
+    <t>ebtsGbWllYg</t>
+  </si>
+  <si>
+    <t>ko Okene</t>
+  </si>
+  <si>
+    <t>ko Nagazi Clinic</t>
+  </si>
+  <si>
+    <t>rlB4mUoaEdr</t>
   </si>
 </sst>
 </file>
@@ -18790,10 +19216,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E1171"/>
+  <dimension ref="A1:E1172"/>
   <sheetViews>
-    <sheetView topLeftCell="A1150" workbookViewId="0">
-      <selection activeCell="B1150" sqref="B1150"/>
+    <sheetView topLeftCell="A1165" workbookViewId="0">
+      <selection activeCell="B1172" sqref="B1172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -35203,6 +35629,20 @@
       </c>
       <c r="D1171" t="s">
         <v>5743</v>
+      </c>
+    </row>
+    <row r="1172" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1172" s="6" t="s">
+        <v>890</v>
+      </c>
+      <c r="B1172" t="s">
+        <v>6046</v>
+      </c>
+      <c r="C1172" t="s">
+        <v>6046</v>
+      </c>
+      <c r="D1172" t="s">
+        <v>6047</v>
       </c>
     </row>
   </sheetData>
@@ -54740,10 +55180,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D198"/>
+  <dimension ref="A1:D199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B198" sqref="B198"/>
+    <sheetView topLeftCell="A187" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C199" sqref="C199:D199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -57424,18 +57864,32 @@
         <v>6045</v>
       </c>
     </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A199" t="s">
+        <v>4412</v>
+      </c>
+      <c r="B199" t="s">
+        <v>2832</v>
+      </c>
+      <c r="C199" t="s">
+        <v>6046</v>
+      </c>
+      <c r="D199" t="s">
+        <v>6047</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D162"/>
   <conditionalFormatting sqref="D229:D1048576 D1:D162">
     <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  <conditionalFormatting sqref="C1:C198 C200:C1048576">
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="D1:D198 D200:D1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -57444,18 +57898,18 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="77.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -57486,6 +57940,818 @@
         <v>6004</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>6048</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6049</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6050</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6051</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>6048</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6052</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6053</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6054</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>6048</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6055</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6056</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6057</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>6048</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6058</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6059</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6060</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>6048</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6061</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6062</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6063</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>6048</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6061</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6064</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6065</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>6048</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6061</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6066</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6067</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>6048</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6061</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6068</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6069</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>6048</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6061</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6070</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6071</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>6048</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6061</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6072</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6073</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>6048</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6061</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6074</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6075</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>6048</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6061</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6076</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6077</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>6048</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6061</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6078</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6079</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>6048</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6080</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6081</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6082</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6083</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6084</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6085</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6083</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6086</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6087</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6083</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6088</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6089</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6083</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6090</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6091</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6092</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6093</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6094</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6005</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6095</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6096</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6005</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6097</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6098</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6005</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6099</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6005</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6101</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6005</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6103</v>
+      </c>
+      <c r="D26" t="s">
+        <v>6104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6105</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6106</v>
+      </c>
+      <c r="D27" t="s">
+        <v>6107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6105</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6108</v>
+      </c>
+      <c r="D28" t="s">
+        <v>6109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6105</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6110</v>
+      </c>
+      <c r="D29" t="s">
+        <v>6111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6105</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6112</v>
+      </c>
+      <c r="D30" t="s">
+        <v>6113</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6114</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6115</v>
+      </c>
+      <c r="D31" t="s">
+        <v>6116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6114</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6117</v>
+      </c>
+      <c r="D32" t="s">
+        <v>6118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6114</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6119</v>
+      </c>
+      <c r="D33" t="s">
+        <v>6120</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6114</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6121</v>
+      </c>
+      <c r="D34" t="s">
+        <v>6122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B35" t="s">
+        <v>6123</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6124</v>
+      </c>
+      <c r="D35" t="s">
+        <v>6125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B36" t="s">
+        <v>6123</v>
+      </c>
+      <c r="C36" t="s">
+        <v>6126</v>
+      </c>
+      <c r="D36" t="s">
+        <v>6127</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B37" t="s">
+        <v>6123</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6128</v>
+      </c>
+      <c r="D37" t="s">
+        <v>6129</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B38" t="s">
+        <v>6130</v>
+      </c>
+      <c r="C38" t="s">
+        <v>6131</v>
+      </c>
+      <c r="D38" t="s">
+        <v>6132</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B39" t="s">
+        <v>6133</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6134</v>
+      </c>
+      <c r="D39" t="s">
+        <v>6135</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B40" t="s">
+        <v>6136</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6137</v>
+      </c>
+      <c r="D40" t="s">
+        <v>6138</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B41" t="s">
+        <v>6136</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6139</v>
+      </c>
+      <c r="D41" t="s">
+        <v>6140</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B42" t="s">
+        <v>6136</v>
+      </c>
+      <c r="C42" t="s">
+        <v>6141</v>
+      </c>
+      <c r="D42" t="s">
+        <v>6142</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B43" t="s">
+        <v>6136</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6143</v>
+      </c>
+      <c r="D43" t="s">
+        <v>6144</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B44" t="s">
+        <v>6145</v>
+      </c>
+      <c r="C44" t="s">
+        <v>6146</v>
+      </c>
+      <c r="D44" t="s">
+        <v>6147</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B45" t="s">
+        <v>6148</v>
+      </c>
+      <c r="C45" t="s">
+        <v>6149</v>
+      </c>
+      <c r="D45" t="s">
+        <v>6150</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B46" t="s">
+        <v>6148</v>
+      </c>
+      <c r="C46" t="s">
+        <v>6151</v>
+      </c>
+      <c r="D46" t="s">
+        <v>6152</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B47" t="s">
+        <v>6148</v>
+      </c>
+      <c r="C47" t="s">
+        <v>6153</v>
+      </c>
+      <c r="D47" t="s">
+        <v>6154</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B48" t="s">
+        <v>6148</v>
+      </c>
+      <c r="C48" t="s">
+        <v>6155</v>
+      </c>
+      <c r="D48" t="s">
+        <v>6156</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B49" t="s">
+        <v>6148</v>
+      </c>
+      <c r="C49" t="s">
+        <v>6157</v>
+      </c>
+      <c r="D49" t="s">
+        <v>6158</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>6159</v>
+      </c>
+      <c r="B50" t="s">
+        <v>6160</v>
+      </c>
+      <c r="C50" t="s">
+        <v>6161</v>
+      </c>
+      <c r="D50" t="s">
+        <v>6162</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>6159</v>
+      </c>
+      <c r="B51" t="s">
+        <v>6160</v>
+      </c>
+      <c r="C51" t="s">
+        <v>6163</v>
+      </c>
+      <c r="D51" t="s">
+        <v>6164</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>6159</v>
+      </c>
+      <c r="B52" t="s">
+        <v>6165</v>
+      </c>
+      <c r="C52" t="s">
+        <v>6166</v>
+      </c>
+      <c r="D52" t="s">
+        <v>6167</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>6159</v>
+      </c>
+      <c r="B53" t="s">
+        <v>6165</v>
+      </c>
+      <c r="C53" t="s">
+        <v>6168</v>
+      </c>
+      <c r="D53" t="s">
+        <v>6169</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>6159</v>
+      </c>
+      <c r="B54" t="s">
+        <v>6165</v>
+      </c>
+      <c r="C54" t="s">
+        <v>6170</v>
+      </c>
+      <c r="D54" t="s">
+        <v>6171</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>6159</v>
+      </c>
+      <c r="B55" t="s">
+        <v>6165</v>
+      </c>
+      <c r="C55" t="s">
+        <v>6172</v>
+      </c>
+      <c r="D55" t="s">
+        <v>6173</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>6159</v>
+      </c>
+      <c r="B56" t="s">
+        <v>6174</v>
+      </c>
+      <c r="C56" t="s">
+        <v>6175</v>
+      </c>
+      <c r="D56" t="s">
+        <v>6176</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>6159</v>
+      </c>
+      <c r="B57" t="s">
+        <v>6174</v>
+      </c>
+      <c r="C57" t="s">
+        <v>6177</v>
+      </c>
+      <c r="D57" t="s">
+        <v>6178</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>6159</v>
+      </c>
+      <c r="B58" t="s">
+        <v>6179</v>
+      </c>
+      <c r="C58" t="s">
+        <v>6180</v>
+      </c>
+      <c r="D58" t="s">
+        <v>6181</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>6159</v>
+      </c>
+      <c r="B59" t="s">
+        <v>6182</v>
+      </c>
+      <c r="C59" t="s">
+        <v>6183</v>
+      </c>
+      <c r="D59" t="s">
+        <v>6184</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>6159</v>
+      </c>
+      <c r="B60" t="s">
+        <v>6185</v>
+      </c>
+      <c r="C60" t="s">
+        <v>6186</v>
+      </c>
+      <c r="D60" t="s">
+        <v>6187</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
MPM and DQA Q4 FY18 update
</commit_message>
<xml_diff>
--- a/DMP/Report/Template/ART sites.xlsx
+++ b/DMP/Report/Template/ART sites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MGIC\Project\ShieldPortal\DMP\Report\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2CD2606A-5DF4-4804-9351-3B2AE9E95897}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5767DA88-EED4-45E3-BF93-86293F216D70}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <definedName name="LGA">[1]MainPage!$S$17</definedName>
     <definedName name="LGAFac_list">[1]!LGAFac[#Headers]</definedName>
   </definedNames>
-  <calcPr calcId="171027" iterate="1" iterateCount="1" iterateDelta="1E-4"/>
+  <calcPr calcId="179017" iterate="1" iterateCount="1" iterateDelta="1E-4"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -19216,8 +19216,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E1171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1002" workbookViewId="0">
-      <selection activeCell="B1014" sqref="B1014"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -35642,8 +35642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:ACT98"/>
   <sheetViews>
-    <sheetView topLeftCell="PB1" workbookViewId="0">
-      <selection activeCell="PD19" sqref="PD19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>